<commit_message>
rerun sat and gurobi approaches
</commit_message>
<xml_diff>
--- a/experiments/nrp_sat_bdd_exp_results.xlsx
+++ b/experiments/nrp_sat_bdd_exp_results.xlsx
@@ -490,10 +490,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0625979</v>
+        <v>0.0615436</v>
       </c>
       <c r="G2" t="n">
-        <v>7.3</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="H2" t="n">
         <v>19084</v>
@@ -521,10 +521,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0626193</v>
+        <v>0.0625984</v>
       </c>
       <c r="G3" t="n">
-        <v>7.1</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="H3" t="n">
         <v>19084</v>
@@ -552,10 +552,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0617761</v>
+        <v>0.061477</v>
       </c>
       <c r="G4" t="n">
-        <v>4.9</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="H4" t="n">
         <v>19084</v>
@@ -583,10 +583,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.06256490000000001</v>
+        <v>0.061504</v>
       </c>
       <c r="G5" t="n">
-        <v>4.9</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="H5" t="n">
         <v>19084</v>
@@ -614,10 +614,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0615764</v>
+        <v>0.0615597</v>
       </c>
       <c r="G6" t="n">
-        <v>7.3</v>
+        <v>8.6</v>
       </c>
       <c r="H6" t="n">
         <v>19084</v>
@@ -645,10 +645,10 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0626244</v>
+        <v>0.0614529</v>
       </c>
       <c r="G7" t="n">
-        <v>7.4</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="H7" t="n">
         <v>19084</v>
@@ -676,10 +676,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0625991</v>
+        <v>0.0615633</v>
       </c>
       <c r="G8" t="n">
-        <v>7.3</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="H8" t="n">
         <v>19084</v>
@@ -707,10 +707,10 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0626187</v>
+        <v>0.0626086</v>
       </c>
       <c r="G9" t="n">
-        <v>7.3</v>
+        <v>9.5</v>
       </c>
       <c r="H9" t="n">
         <v>19084</v>
@@ -738,10 +738,10 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0626311</v>
+        <v>0.0625894</v>
       </c>
       <c r="G10" t="n">
-        <v>7.2</v>
+        <v>9.5</v>
       </c>
       <c r="H10" t="n">
         <v>19084</v>
@@ -769,10 +769,10 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0615079</v>
+        <v>0.0626419</v>
       </c>
       <c r="G11" t="n">
-        <v>7.3</v>
+        <v>9.5</v>
       </c>
       <c r="H11" t="n">
         <v>19084</v>
@@ -802,10 +802,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.06231158</v>
+        <v>0.06195388</v>
       </c>
       <c r="G12" t="n">
-        <v>6.8</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="H12" t="n">
         <v>19084</v>
@@ -899,10 +899,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.107741</v>
+        <v>0.108558</v>
       </c>
       <c r="G2" t="n">
-        <v>7.3</v>
+        <v>15.7</v>
       </c>
       <c r="H2" t="n">
         <v>36084</v>
@@ -930,10 +930,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.108749</v>
+        <v>0.107557</v>
       </c>
       <c r="G3" t="n">
-        <v>7.2</v>
+        <v>15.6</v>
       </c>
       <c r="H3" t="n">
         <v>36084</v>
@@ -961,10 +961,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.108578</v>
+        <v>0.107399</v>
       </c>
       <c r="G4" t="n">
-        <v>4.9</v>
+        <v>15.7</v>
       </c>
       <c r="H4" t="n">
         <v>36084</v>
@@ -992,10 +992,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.108566</v>
+        <v>0.110661</v>
       </c>
       <c r="G5" t="n">
-        <v>7.3</v>
+        <v>15.7</v>
       </c>
       <c r="H5" t="n">
         <v>36084</v>
@@ -1023,10 +1023,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.108611</v>
+        <v>0.108539</v>
       </c>
       <c r="G6" t="n">
-        <v>7.1</v>
+        <v>15.7</v>
       </c>
       <c r="H6" t="n">
         <v>36084</v>
@@ -1054,10 +1054,10 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.10847</v>
+        <v>0.107461</v>
       </c>
       <c r="G7" t="n">
-        <v>7.3</v>
+        <v>15.7</v>
       </c>
       <c r="H7" t="n">
         <v>36084</v>
@@ -1085,10 +1085,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.108588</v>
+        <v>0.109457</v>
       </c>
       <c r="G8" t="n">
-        <v>4.9</v>
+        <v>15.7</v>
       </c>
       <c r="H8" t="n">
         <v>36084</v>
@@ -1116,10 +1116,10 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.110694</v>
+        <v>0.109663</v>
       </c>
       <c r="G9" t="n">
-        <v>7.3</v>
+        <v>15.7</v>
       </c>
       <c r="H9" t="n">
         <v>36084</v>
@@ -1147,10 +1147,10 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.107463</v>
+        <v>0.109648</v>
       </c>
       <c r="G10" t="n">
-        <v>5</v>
+        <v>15.7</v>
       </c>
       <c r="H10" t="n">
         <v>36084</v>
@@ -1178,10 +1178,10 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.108467</v>
+        <v>0.107345</v>
       </c>
       <c r="G11" t="n">
-        <v>7.4</v>
+        <v>15.7</v>
       </c>
       <c r="H11" t="n">
         <v>36084</v>
@@ -1211,10 +1211,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1085927</v>
+        <v>0.1086288</v>
       </c>
       <c r="G12" t="n">
-        <v>6.57</v>
+        <v>15.69</v>
       </c>
       <c r="H12" t="n">
         <v>36084</v>
@@ -1308,10 +1308,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.157666</v>
+        <v>0.155685</v>
       </c>
       <c r="G2" t="n">
-        <v>20.9</v>
+        <v>23</v>
       </c>
       <c r="H2" t="n">
         <v>53084</v>
@@ -1339,10 +1339,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.157775</v>
+        <v>0.156682</v>
       </c>
       <c r="G3" t="n">
-        <v>20.6</v>
+        <v>23.6</v>
       </c>
       <c r="H3" t="n">
         <v>53084</v>
@@ -1370,10 +1370,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.157851</v>
+        <v>0.156595</v>
       </c>
       <c r="G4" t="n">
-        <v>20.6</v>
+        <v>23</v>
       </c>
       <c r="H4" t="n">
         <v>53084</v>
@@ -1401,10 +1401,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.155441</v>
+        <v>0.154424</v>
       </c>
       <c r="G5" t="n">
-        <v>21.5</v>
+        <v>23.6</v>
       </c>
       <c r="H5" t="n">
         <v>53084</v>
@@ -1432,10 +1432,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.158894</v>
+        <v>0.15968</v>
       </c>
       <c r="G6" t="n">
-        <v>20.8</v>
+        <v>23.2</v>
       </c>
       <c r="H6" t="n">
         <v>53084</v>
@@ -1463,10 +1463,10 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.159302</v>
+        <v>0.155954</v>
       </c>
       <c r="G7" t="n">
-        <v>20.7</v>
+        <v>23.4</v>
       </c>
       <c r="H7" t="n">
         <v>53084</v>
@@ -1494,10 +1494,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.157699</v>
+        <v>0.156764</v>
       </c>
       <c r="G8" t="n">
-        <v>20.8</v>
+        <v>23</v>
       </c>
       <c r="H8" t="n">
         <v>53084</v>
@@ -1525,10 +1525,10 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.160459</v>
+        <v>0.157574</v>
       </c>
       <c r="G9" t="n">
-        <v>21.3</v>
+        <v>23.3</v>
       </c>
       <c r="H9" t="n">
         <v>53084</v>
@@ -1556,10 +1556,10 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.155518</v>
+        <v>0.156624</v>
       </c>
       <c r="G10" t="n">
-        <v>21.5</v>
+        <v>23</v>
       </c>
       <c r="H10" t="n">
         <v>53084</v>
@@ -1587,10 +1587,10 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.159766</v>
+        <v>0.160933</v>
       </c>
       <c r="G11" t="n">
-        <v>20.7</v>
+        <v>23.2</v>
       </c>
       <c r="H11" t="n">
         <v>53084</v>
@@ -1620,10 +1620,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1580371</v>
+        <v>0.1570915</v>
       </c>
       <c r="G12" t="n">
-        <v>20.94</v>
+        <v>23.23</v>
       </c>
       <c r="H12" t="n">
         <v>53084</v>
@@ -1717,10 +1717,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.204749</v>
+        <v>0.203614</v>
       </c>
       <c r="G2" t="n">
-        <v>21.4</v>
+        <v>27.1</v>
       </c>
       <c r="H2" t="n">
         <v>70084</v>
@@ -1748,10 +1748,10 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.203765</v>
+        <v>0.201235</v>
       </c>
       <c r="G3" t="n">
-        <v>20.9</v>
+        <v>27.7</v>
       </c>
       <c r="H3" t="n">
         <v>70084</v>
@@ -1779,10 +1779,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.202729</v>
+        <v>0.20126</v>
       </c>
       <c r="G4" t="n">
-        <v>21.4</v>
+        <v>27.6</v>
       </c>
       <c r="H4" t="n">
         <v>70084</v>
@@ -1810,10 +1810,10 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.201518</v>
+        <v>0.200355</v>
       </c>
       <c r="G5" t="n">
-        <v>21.5</v>
+        <v>28.5</v>
       </c>
       <c r="H5" t="n">
         <v>70084</v>
@@ -1841,10 +1841,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.204553</v>
+        <v>0.203542</v>
       </c>
       <c r="G6" t="n">
-        <v>21.6</v>
+        <v>28.9</v>
       </c>
       <c r="H6" t="n">
         <v>70084</v>
@@ -1872,10 +1872,10 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.202363</v>
+        <v>0.201133</v>
       </c>
       <c r="G7" t="n">
-        <v>21.6</v>
+        <v>27.8</v>
       </c>
       <c r="H7" t="n">
         <v>70084</v>
@@ -1903,10 +1903,10 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.203368</v>
+        <v>0.202215</v>
       </c>
       <c r="G8" t="n">
-        <v>21.5</v>
+        <v>27.5</v>
       </c>
       <c r="H8" t="n">
         <v>70084</v>
@@ -1934,10 +1934,10 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.201382</v>
+        <v>0.204395</v>
       </c>
       <c r="G9" t="n">
-        <v>21.4</v>
+        <v>27.9</v>
       </c>
       <c r="H9" t="n">
         <v>70084</v>
@@ -1965,10 +1965,10 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.202445</v>
+        <v>0.201762</v>
       </c>
       <c r="G10" t="n">
-        <v>21.6</v>
+        <v>28.3</v>
       </c>
       <c r="H10" t="n">
         <v>70084</v>
@@ -1996,10 +1996,10 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.203133</v>
+        <v>0.203813</v>
       </c>
       <c r="G11" t="n">
-        <v>20.9</v>
+        <v>27.9</v>
       </c>
       <c r="H11" t="n">
         <v>70084</v>
@@ -2029,10 +2029,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2030005</v>
+        <v>0.2023324</v>
       </c>
       <c r="G12" t="n">
-        <v>21.38</v>
+        <v>27.92</v>
       </c>
       <c r="H12" t="n">
         <v>70084</v>

</xml_diff>

<commit_message>
only measure encoding and solving time of sat approaches & rerun
</commit_message>
<xml_diff>
--- a/experiments/nrp_sat_bdd_exp_results.xlsx
+++ b/experiments/nrp_sat_bdd_exp_results.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,20 +452,30 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>wall_time_sec</t>
+          <t>encoding_time_sec</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>solving_time_sec</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>total_time_sec</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>peak_memory_mb</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>total_clauses</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>total_variables</t>
         </is>
@@ -490,17 +500,19 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0615436</v>
+        <v>0.0476336</v>
       </c>
       <c r="G2" t="n">
-        <v>8.699999999999999</v>
+        <v>0.0033069</v>
       </c>
       <c r="H2" t="n">
-        <v>19084</v>
+        <v>0.0509405</v>
       </c>
       <c r="I2" t="n">
-        <v>10268</v>
-      </c>
+        <v>9.800000000000001</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -521,17 +533,19 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0625984</v>
+        <v>0.0464272</v>
       </c>
       <c r="G3" t="n">
+        <v>0.00271281</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.04914</v>
+      </c>
+      <c r="I3" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="H3" t="n">
-        <v>19084</v>
-      </c>
-      <c r="I3" t="n">
-        <v>10268</v>
-      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -552,17 +566,19 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.061477</v>
+        <v>0.0459506</v>
       </c>
       <c r="G4" t="n">
+        <v>0.0026963</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0486469</v>
+      </c>
+      <c r="I4" t="n">
         <v>8.699999999999999</v>
       </c>
-      <c r="H4" t="n">
-        <v>19084</v>
-      </c>
-      <c r="I4" t="n">
-        <v>10268</v>
-      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -583,17 +599,19 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.061504</v>
+        <v>0.0467455</v>
       </c>
       <c r="G5" t="n">
+        <v>0.0032264</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0499719</v>
+      </c>
+      <c r="I5" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="H5" t="n">
-        <v>19084</v>
-      </c>
-      <c r="I5" t="n">
-        <v>10268</v>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -614,17 +632,19 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0615597</v>
+        <v>0.0468162</v>
       </c>
       <c r="G6" t="n">
-        <v>8.6</v>
+        <v>0.00274581</v>
       </c>
       <c r="H6" t="n">
-        <v>19084</v>
+        <v>0.049562</v>
       </c>
       <c r="I6" t="n">
-        <v>10268</v>
-      </c>
+        <v>8.5</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -645,17 +665,19 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0614529</v>
+        <v>0.0460983</v>
       </c>
       <c r="G7" t="n">
-        <v>8.699999999999999</v>
+        <v>0.00237766</v>
       </c>
       <c r="H7" t="n">
-        <v>19084</v>
+        <v>0.0484759</v>
       </c>
       <c r="I7" t="n">
-        <v>10268</v>
-      </c>
+        <v>8.800000000000001</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -676,17 +698,19 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0615633</v>
+        <v>0.0479079</v>
       </c>
       <c r="G8" t="n">
-        <v>8.699999999999999</v>
+        <v>0.00304461</v>
       </c>
       <c r="H8" t="n">
-        <v>19084</v>
+        <v>0.0509525</v>
       </c>
       <c r="I8" t="n">
-        <v>10268</v>
-      </c>
+        <v>9.800000000000001</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -707,17 +731,19 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0626086</v>
+        <v>0.048095</v>
       </c>
       <c r="G9" t="n">
-        <v>9.5</v>
+        <v>0.00254395</v>
       </c>
       <c r="H9" t="n">
-        <v>19084</v>
+        <v>0.050639</v>
       </c>
       <c r="I9" t="n">
-        <v>10268</v>
-      </c>
+        <v>8.300000000000001</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -738,17 +764,19 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0625894</v>
+        <v>0.0455709</v>
       </c>
       <c r="G10" t="n">
-        <v>9.5</v>
+        <v>0.00236888</v>
       </c>
       <c r="H10" t="n">
-        <v>19084</v>
+        <v>0.0479398</v>
       </c>
       <c r="I10" t="n">
-        <v>10268</v>
-      </c>
+        <v>8.800000000000001</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -769,17 +797,19 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0626419</v>
+        <v>0.0456859</v>
       </c>
       <c r="G11" t="n">
-        <v>9.5</v>
+        <v>0.0025821</v>
       </c>
       <c r="H11" t="n">
-        <v>19084</v>
+        <v>0.048268</v>
       </c>
       <c r="I11" t="n">
-        <v>10268</v>
-      </c>
+        <v>8.699999999999999</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -802,17 +832,19 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.06195388</v>
+        <v>0.04669311</v>
       </c>
       <c r="G12" t="n">
-        <v>8.949999999999999</v>
+        <v>0.002760542</v>
       </c>
       <c r="H12" t="n">
-        <v>19084</v>
+        <v>0.04945365</v>
       </c>
       <c r="I12" t="n">
-        <v>10268</v>
-      </c>
+        <v>8.9</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -825,7 +857,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -861,20 +893,30 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>wall_time_sec</t>
+          <t>encoding_time_sec</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>solving_time_sec</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>total_time_sec</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>peak_memory_mb</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>total_clauses</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>total_variables</t>
         </is>
@@ -899,17 +941,19 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.108558</v>
+        <v>0.0890898</v>
       </c>
       <c r="G2" t="n">
+        <v>0.00583576</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.0949255</v>
+      </c>
+      <c r="I2" t="n">
         <v>15.7</v>
       </c>
-      <c r="H2" t="n">
-        <v>36084</v>
-      </c>
-      <c r="I2" t="n">
-        <v>19308</v>
-      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -930,17 +974,19 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.107557</v>
+        <v>0.0885563</v>
       </c>
       <c r="G3" t="n">
-        <v>15.6</v>
+        <v>0.0051259</v>
       </c>
       <c r="H3" t="n">
-        <v>36084</v>
+        <v>0.0936823</v>
       </c>
       <c r="I3" t="n">
-        <v>19308</v>
-      </c>
+        <v>15.7</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -961,17 +1007,19 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.107399</v>
+        <v>0.0871721</v>
       </c>
       <c r="G4" t="n">
-        <v>15.7</v>
+        <v>0.00400175</v>
       </c>
       <c r="H4" t="n">
-        <v>36084</v>
+        <v>0.0911739</v>
       </c>
       <c r="I4" t="n">
-        <v>19308</v>
-      </c>
+        <v>14.5</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -992,17 +1040,19 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.110661</v>
+        <v>0.09026240000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>15.7</v>
+        <v>0.00566894</v>
       </c>
       <c r="H5" t="n">
-        <v>36084</v>
+        <v>0.0959313</v>
       </c>
       <c r="I5" t="n">
-        <v>19308</v>
-      </c>
+        <v>15.1</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1023,17 +1073,19 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.108539</v>
+        <v>0.09051720000000001</v>
       </c>
       <c r="G6" t="n">
-        <v>15.7</v>
+        <v>0.00521189</v>
       </c>
       <c r="H6" t="n">
-        <v>36084</v>
+        <v>0.0957291</v>
       </c>
       <c r="I6" t="n">
-        <v>19308</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1054,17 +1106,19 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.107461</v>
+        <v>0.0866788</v>
       </c>
       <c r="G7" t="n">
-        <v>15.7</v>
+        <v>0.00407781</v>
       </c>
       <c r="H7" t="n">
-        <v>36084</v>
+        <v>0.09075660000000001</v>
       </c>
       <c r="I7" t="n">
-        <v>19308</v>
-      </c>
+        <v>14.5</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1085,17 +1139,19 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.109457</v>
+        <v>0.08821420000000001</v>
       </c>
       <c r="G8" t="n">
+        <v>0.00450065</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0927148</v>
+      </c>
+      <c r="I8" t="n">
         <v>15.7</v>
       </c>
-      <c r="H8" t="n">
-        <v>36084</v>
-      </c>
-      <c r="I8" t="n">
-        <v>19308</v>
-      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1116,17 +1172,19 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.109663</v>
+        <v>0.0911633</v>
       </c>
       <c r="G9" t="n">
-        <v>15.7</v>
+        <v>0.00635459</v>
       </c>
       <c r="H9" t="n">
-        <v>36084</v>
+        <v>0.0975178</v>
       </c>
       <c r="I9" t="n">
-        <v>19308</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1147,17 +1205,19 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.109648</v>
+        <v>0.0892155</v>
       </c>
       <c r="G10" t="n">
-        <v>15.7</v>
+        <v>0.0055552</v>
       </c>
       <c r="H10" t="n">
-        <v>36084</v>
+        <v>0.0947707</v>
       </c>
       <c r="I10" t="n">
-        <v>19308</v>
-      </c>
+        <v>15.1</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1178,17 +1238,19 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.107345</v>
+        <v>0.0873261</v>
       </c>
       <c r="G11" t="n">
+        <v>0.00400778</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0913339</v>
+      </c>
+      <c r="I11" t="n">
         <v>15.7</v>
       </c>
-      <c r="H11" t="n">
-        <v>36084</v>
-      </c>
-      <c r="I11" t="n">
-        <v>19308</v>
-      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1211,17 +1273,19 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1086288</v>
+        <v>0.08881957</v>
       </c>
       <c r="G12" t="n">
-        <v>15.69</v>
+        <v>0.005034027000000001</v>
       </c>
       <c r="H12" t="n">
-        <v>36084</v>
+        <v>0.09385359</v>
       </c>
       <c r="I12" t="n">
-        <v>19308</v>
-      </c>
+        <v>15.2</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1234,7 +1298,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1270,20 +1334,30 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>wall_time_sec</t>
+          <t>encoding_time_sec</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>solving_time_sec</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>total_time_sec</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>peak_memory_mb</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>total_clauses</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>total_variables</t>
         </is>
@@ -1308,17 +1382,19 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.155685</v>
+        <v>0.132824</v>
       </c>
       <c r="G2" t="n">
-        <v>23</v>
+        <v>0.007902299999999999</v>
       </c>
       <c r="H2" t="n">
-        <v>53084</v>
+        <v>0.140727</v>
       </c>
       <c r="I2" t="n">
-        <v>28348</v>
-      </c>
+        <v>22.1</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1339,17 +1415,19 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.156682</v>
+        <v>0.134056</v>
       </c>
       <c r="G3" t="n">
-        <v>23.6</v>
+        <v>0.00788706</v>
       </c>
       <c r="H3" t="n">
-        <v>53084</v>
+        <v>0.141943</v>
       </c>
       <c r="I3" t="n">
-        <v>28348</v>
-      </c>
+        <v>22.1</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1370,17 +1448,19 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.156595</v>
+        <v>0.138109</v>
       </c>
       <c r="G4" t="n">
-        <v>23</v>
+        <v>0.008206130000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>53084</v>
+        <v>0.146315</v>
       </c>
       <c r="I4" t="n">
-        <v>28348</v>
-      </c>
+        <v>23.2</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1401,17 +1481,19 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.154424</v>
+        <v>0.132919</v>
       </c>
       <c r="G5" t="n">
-        <v>23.6</v>
+        <v>0.00700027</v>
       </c>
       <c r="H5" t="n">
-        <v>53084</v>
+        <v>0.13992</v>
       </c>
       <c r="I5" t="n">
-        <v>28348</v>
-      </c>
+        <v>22.4</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1432,17 +1514,19 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.15968</v>
+        <v>0.136478</v>
       </c>
       <c r="G6" t="n">
-        <v>23.2</v>
+        <v>0.008356199999999999</v>
       </c>
       <c r="H6" t="n">
-        <v>53084</v>
+        <v>0.144834</v>
       </c>
       <c r="I6" t="n">
-        <v>28348</v>
-      </c>
+        <v>23.6</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1463,17 +1547,19 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.155954</v>
+        <v>0.144364</v>
       </c>
       <c r="G7" t="n">
-        <v>23.4</v>
+        <v>0.00856986</v>
       </c>
       <c r="H7" t="n">
-        <v>53084</v>
+        <v>0.152934</v>
       </c>
       <c r="I7" t="n">
-        <v>28348</v>
-      </c>
+        <v>23.6</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1494,17 +1580,19 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.156764</v>
+        <v>0.139338</v>
       </c>
       <c r="G8" t="n">
-        <v>23</v>
+        <v>0.009078650000000001</v>
       </c>
       <c r="H8" t="n">
-        <v>53084</v>
+        <v>0.148417</v>
       </c>
       <c r="I8" t="n">
-        <v>28348</v>
-      </c>
+        <v>23.3</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1525,17 +1613,19 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.157574</v>
+        <v>0.137298</v>
       </c>
       <c r="G9" t="n">
-        <v>23.3</v>
+        <v>0.00774202</v>
       </c>
       <c r="H9" t="n">
-        <v>53084</v>
+        <v>0.14504</v>
       </c>
       <c r="I9" t="n">
-        <v>28348</v>
-      </c>
+        <v>23.6</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1556,17 +1646,19 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.156624</v>
+        <v>0.138809</v>
       </c>
       <c r="G10" t="n">
-        <v>23</v>
+        <v>0.00800993</v>
       </c>
       <c r="H10" t="n">
-        <v>53084</v>
+        <v>0.146819</v>
       </c>
       <c r="I10" t="n">
-        <v>28348</v>
-      </c>
+        <v>23.3</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1587,17 +1679,19 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.160933</v>
+        <v>0.138587</v>
       </c>
       <c r="G11" t="n">
-        <v>23.2</v>
+        <v>0.00820309</v>
       </c>
       <c r="H11" t="n">
-        <v>53084</v>
+        <v>0.14679</v>
       </c>
       <c r="I11" t="n">
-        <v>28348</v>
-      </c>
+        <v>23.3</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1620,17 +1714,19 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.1570915</v>
+        <v>0.1372782</v>
       </c>
       <c r="G12" t="n">
-        <v>23.23</v>
+        <v>0.008095550999999999</v>
       </c>
       <c r="H12" t="n">
-        <v>53084</v>
+        <v>0.1453739</v>
       </c>
       <c r="I12" t="n">
-        <v>28348</v>
-      </c>
+        <v>23.05</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1643,7 +1739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1679,20 +1775,30 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>wall_time_sec</t>
+          <t>encoding_time_sec</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>solving_time_sec</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>total_time_sec</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
           <t>peak_memory_mb</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>total_clauses</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>total_variables</t>
         </is>
@@ -1717,17 +1823,19 @@
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.203614</v>
+        <v>0.174549</v>
       </c>
       <c r="G2" t="n">
-        <v>27.1</v>
+        <v>0.0100449</v>
       </c>
       <c r="H2" t="n">
-        <v>70084</v>
+        <v>0.184594</v>
       </c>
       <c r="I2" t="n">
-        <v>37388</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1748,17 +1856,19 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.201235</v>
+        <v>0.173385</v>
       </c>
       <c r="G3" t="n">
-        <v>27.7</v>
+        <v>0.0102257</v>
       </c>
       <c r="H3" t="n">
-        <v>70084</v>
+        <v>0.18361</v>
       </c>
       <c r="I3" t="n">
-        <v>37388</v>
-      </c>
+        <v>27.5</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1779,17 +1889,19 @@
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.20126</v>
+        <v>0.176883</v>
       </c>
       <c r="G4" t="n">
-        <v>27.6</v>
+        <v>0.0101787</v>
       </c>
       <c r="H4" t="n">
-        <v>70084</v>
+        <v>0.187062</v>
       </c>
       <c r="I4" t="n">
-        <v>37388</v>
-      </c>
+        <v>28.6</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1810,17 +1922,19 @@
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.200355</v>
+        <v>0.175848</v>
       </c>
       <c r="G5" t="n">
-        <v>28.5</v>
+        <v>0.009375619999999999</v>
       </c>
       <c r="H5" t="n">
-        <v>70084</v>
+        <v>0.185224</v>
       </c>
       <c r="I5" t="n">
-        <v>37388</v>
-      </c>
+        <v>28.3</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1841,17 +1955,19 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>0.203542</v>
+        <v>0.17814</v>
       </c>
       <c r="G6" t="n">
-        <v>28.9</v>
+        <v>0.0108777</v>
       </c>
       <c r="H6" t="n">
-        <v>70084</v>
+        <v>0.189018</v>
       </c>
       <c r="I6" t="n">
-        <v>37388</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1872,17 +1988,19 @@
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>0.201133</v>
+        <v>0.175022</v>
       </c>
       <c r="G7" t="n">
-        <v>27.8</v>
+        <v>0.0109945</v>
       </c>
       <c r="H7" t="n">
-        <v>70084</v>
+        <v>0.186017</v>
       </c>
       <c r="I7" t="n">
-        <v>37388</v>
-      </c>
+        <v>27.7</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1903,17 +2021,19 @@
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.202215</v>
+        <v>0.177476</v>
       </c>
       <c r="G8" t="n">
-        <v>27.5</v>
+        <v>0.0113741</v>
       </c>
       <c r="H8" t="n">
-        <v>70084</v>
+        <v>0.18885</v>
       </c>
       <c r="I8" t="n">
-        <v>37388</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1934,17 +2054,19 @@
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.204395</v>
+        <v>0.181928</v>
       </c>
       <c r="G9" t="n">
-        <v>27.9</v>
+        <v>0.0107158</v>
       </c>
       <c r="H9" t="n">
-        <v>70084</v>
+        <v>0.192644</v>
       </c>
       <c r="I9" t="n">
-        <v>37388</v>
-      </c>
+        <v>27.5</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1965,17 +2087,19 @@
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.201762</v>
+        <v>0.177871</v>
       </c>
       <c r="G10" t="n">
-        <v>28.3</v>
+        <v>0.0104599</v>
       </c>
       <c r="H10" t="n">
-        <v>70084</v>
+        <v>0.188331</v>
       </c>
       <c r="I10" t="n">
-        <v>37388</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1996,17 +2120,19 @@
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.203813</v>
+        <v>0.178217</v>
       </c>
       <c r="G11" t="n">
-        <v>27.9</v>
+        <v>0.0110176</v>
       </c>
       <c r="H11" t="n">
-        <v>70084</v>
+        <v>0.189235</v>
       </c>
       <c r="I11" t="n">
-        <v>37388</v>
-      </c>
+        <v>28.2</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -2029,17 +2155,19 @@
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2023324</v>
+        <v>0.1769319</v>
       </c>
       <c r="G12" t="n">
-        <v>27.92</v>
+        <v>0.010526452</v>
       </c>
       <c r="H12" t="n">
-        <v>70084</v>
+        <v>0.1874585</v>
       </c>
       <c r="I12" t="n">
-        <v>37388</v>
-      </c>
+        <v>27.98</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>